<commit_message>
Update: power tolerance analysis completed (kinda)
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5D0C61-CED0-4690-A61A-23C1C9480F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87BC205-2F4D-48A3-BEE4-719AD9F61326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="495" windowWidth="16815" windowHeight="15090" tabRatio="729" firstSheet="7" activeTab="10" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="26340" yWindow="75" windowWidth="11985" windowHeight="13890" tabRatio="729" firstSheet="4" activeTab="10" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="85">
   <si>
     <t>E (eV)</t>
   </si>
@@ -316,6 +316,18 @@
   </si>
   <si>
     <t>111-311</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>111-220</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HHLM spatial chirp (meV/um)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HHLM bandwidth (meV)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2546,10 +2558,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD56799-D342-4B40-B7BD-BBBEDC8F0C10}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3209,6 +3221,22 @@
         <v>1.8045843006325168E-2</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="8">
+        <v>-1.1375067569572901E-18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32">
+        <v>142.46559719211601</v>
+      </c>
+    </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
@@ -3449,6 +3477,22 @@
         <v>1.8045843006325168E-2</v>
       </c>
     </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41">
+        <v>-3.6051209103971797E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42">
+        <v>213.240960670487</v>
+      </c>
+    </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
@@ -3688,6 +3732,22 @@
         <v>1.822998426149175E-2</v>
       </c>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51">
+        <v>-2.5223707918536498E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52">
+        <v>223.86280141900701</v>
+      </c>
+    </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>81</v>
@@ -3925,6 +3985,277 @@
       <c r="I60">
         <f t="shared" si="27"/>
         <v>1.8414125516658331E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="8">
+        <v>-1.1375067569572901E-18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62">
+        <v>223.86280141900701</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" t="s">
+        <v>76</v>
+      </c>
+      <c r="F64" t="s">
+        <v>75</v>
+      </c>
+      <c r="G64" t="s">
+        <v>74</v>
+      </c>
+      <c r="H64" t="s">
+        <v>77</v>
+      </c>
+      <c r="I64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>12.0368582999333</v>
+      </c>
+      <c r="C65">
+        <v>9</v>
+      </c>
+      <c r="D65">
+        <f>SIN(RADIANS(B65-C65))/SIN(RADIANS(B65+C65))</f>
+        <v>0.14758501191458828</v>
+      </c>
+      <c r="E65">
+        <f>A$11/1000</f>
+        <v>9.4809999999999999</v>
+      </c>
+      <c r="F65">
+        <v>3.35</v>
+      </c>
+      <c r="G65">
+        <f>50*0.95^2</f>
+        <v>45.125</v>
+      </c>
+      <c r="H65">
+        <f>G65*F65/E65*0.95</f>
+        <v>15.147169338677356</v>
+      </c>
+      <c r="I65">
+        <f>G65-H65</f>
+        <v>29.977830661322642</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <f>B65</f>
+        <v>12.0368582999333</v>
+      </c>
+      <c r="C66">
+        <f>-C65</f>
+        <v>-9</v>
+      </c>
+      <c r="D66">
+        <f>SIN(RADIANS(B66-C66))/SIN(RADIANS(B66+C66))</f>
+        <v>6.7757557967927591</v>
+      </c>
+      <c r="E66">
+        <f>F65</f>
+        <v>3.35</v>
+      </c>
+      <c r="F66">
+        <v>3.2509999999999999</v>
+      </c>
+      <c r="G66">
+        <f>H65</f>
+        <v>15.147169338677356</v>
+      </c>
+      <c r="H66">
+        <f t="shared" ref="H66:H70" si="28">G66*F66/E66*0.95</f>
+        <v>13.964559744488978</v>
+      </c>
+      <c r="I66">
+        <f>G66-H66</f>
+        <v>1.1826095941883779</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>19.91</v>
+      </c>
+      <c r="C67">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D70" si="29">SIN(RADIANS(B67-C67))/SIN(RADIANS(B67+C67))</f>
+        <v>8.7639288616412861E-2</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E70" si="30">F66</f>
+        <v>3.2509999999999999</v>
+      </c>
+      <c r="F67">
+        <v>1.891</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G70" si="31">H66</f>
+        <v>13.964559744488978</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="28"/>
+        <v>7.7165897732965938</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I70" si="32">G67-H67</f>
+        <v>6.2479699711923846</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <f>B67</f>
+        <v>19.91</v>
+      </c>
+      <c r="C68">
+        <f>-C67</f>
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="29"/>
+        <v>11.410407544233792</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="30"/>
+        <v>1.891</v>
+      </c>
+      <c r="F68">
+        <v>1.8280000000000001</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="31"/>
+        <v>7.7165897732965938</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="28"/>
+        <v>7.0865308304108225</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="32"/>
+        <v>0.63005894288577124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <f>C5</f>
+        <v>42.929010627216698</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="30"/>
+        <v>1.8280000000000001</v>
+      </c>
+      <c r="F69">
+        <v>0.1</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="31"/>
+        <v>7.0865308304108225</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="28"/>
+        <v>0.36828251033316639</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="32"/>
+        <v>6.7182483200776559</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <f>B69</f>
+        <v>42.929010627216698</v>
+      </c>
+      <c r="C70">
+        <v>-15</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="29"/>
+        <v>1.8092059522717598</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="30"/>
+        <v>0.1</v>
+      </c>
+      <c r="F70">
+        <v>0.1</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="31"/>
+        <v>0.36828251033316639</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="28"/>
+        <v>0.34986838481650806</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="32"/>
+        <v>1.8414125516658331E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71">
+        <v>6.77647058825995E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72">
+        <v>66.333555879288298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: new simulations for 17795eV and some updates for the phase corrector
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87BC205-2F4D-48A3-BEE4-719AD9F61326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC6409-969E-4F1A-BC0D-AAE02144EE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26340" yWindow="75" windowWidth="11985" windowHeight="13890" tabRatio="729" firstSheet="4" activeTab="10" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="729" firstSheet="4" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="2DCM-111-440" sheetId="11" r:id="rId9"/>
     <sheet name="2DCM-111-333" sheetId="12" r:id="rId10"/>
     <sheet name="bw factor" sheetId="13" r:id="rId11"/>
+    <sheet name="17795" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="86">
   <si>
     <t>E (eV)</t>
   </si>
@@ -328,6 +329,10 @@
   </si>
   <si>
     <t>HHLM bandwidth (meV)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>111-220-555</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2560,8 +2565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD56799-D342-4B40-B7BD-BBBEDC8F0C10}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4256,6 +4261,506 @@
       </c>
       <c r="C72">
         <v>66.333555879288298</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DF6462-A788-4188-BCB4-115117FE54BC}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>6.38</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>SIN(RADIANS(B2-C2))/SIN(RADIANS(B2+C2))</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>17.795000000000002</v>
+      </c>
+      <c r="F2">
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="G2">
+        <f>40*0.95^2</f>
+        <v>36.1</v>
+      </c>
+      <c r="H2">
+        <f>G2*F2/E2*0.95</f>
+        <v>5.2343478505198089</v>
+      </c>
+      <c r="I2">
+        <f>G2-H2</f>
+        <v>30.865652149480191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <f>B2</f>
+        <v>6.38</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>SIN(RADIANS(B3-C3))/SIN(RADIANS(B3+C3))</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>F2</f>
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="F3">
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="G3">
+        <f>H2</f>
+        <v>5.2343478505198089</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">G3*F3/E3*0.95</f>
+        <v>4.9726304579938185</v>
+      </c>
+      <c r="I3">
+        <f>G3-H3</f>
+        <v>0.26171739252599036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>10.454000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="1">SIN(RADIANS(B4-C4))/SIN(RADIANS(B4+C4))</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E7" si="2">F3</f>
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="F4">
+        <v>1.163</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G7" si="3">H3</f>
+        <v>4.9726304579938185</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.0228316500421468</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I7" si="4">G4-H4</f>
+        <v>2.9497988079516717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <f>B4</f>
+        <v>10.454000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>1.163</v>
+      </c>
+      <c r="F5">
+        <v>1.163</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>2.0228316500421468</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.9216900675400395</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>0.10114158250210736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6">
+        <v>33.747</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>1.163</v>
+      </c>
+      <c r="F6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>1.9216900675400395</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.7895015848201739</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>0.13218848271986561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
+        <f>B6</f>
+        <v>33.747</v>
+      </c>
+      <c r="C7">
+        <v>-15</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2.3392313239218812</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F7">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1.7895015848201739</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.7000265055791648</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>8.9475079241009059E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>6.38</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f>SIN(RADIANS(B12-C12))/SIN(RADIANS(B12+C12))</f>
+        <v>0.36174591529536387</v>
+      </c>
+      <c r="E12">
+        <v>17.795000000000002</v>
+      </c>
+      <c r="F12">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="G12">
+        <f>40*0.95^2</f>
+        <v>36.1</v>
+      </c>
+      <c r="H12">
+        <f>G12*F12/E12*0.95</f>
+        <v>12.92205535262714</v>
+      </c>
+      <c r="I12">
+        <f>G12-H12</f>
+        <v>23.177944647372861</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13">
+        <f>B12</f>
+        <v>6.38</v>
+      </c>
+      <c r="C13">
+        <f>-C12</f>
+        <v>-3</v>
+      </c>
+      <c r="D13">
+        <f>SIN(RADIANS(B13-C13))/SIN(RADIANS(B13+C13))</f>
+        <v>2.764371227753891</v>
+      </c>
+      <c r="E13">
+        <f>F12</f>
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="F13">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="G13">
+        <f>H12</f>
+        <v>12.92205535262714</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H17" si="5">G13*F13/E13*0.95</f>
+        <v>12.275952584995782</v>
+      </c>
+      <c r="I13">
+        <f>G13-H13</f>
+        <v>0.64610276763135843</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>10.454000000000001</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D17" si="6">SIN(RADIANS(B14-C14))/SIN(RADIANS(B14+C14))</f>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E17" si="7">F13</f>
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="F14">
+        <v>2.8330000000000002</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G17" si="8">H13</f>
+        <v>12.275952584995782</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>4.9274996255970764</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I17" si="9">G14-H14</f>
+        <v>7.3484529593987054</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <f>B14</f>
+        <v>10.454000000000001</v>
+      </c>
+      <c r="C15">
+        <f>-C14</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>2.8330000000000002</v>
+      </c>
+      <c r="F15">
+        <v>2.8330000000000002</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="8"/>
+        <v>4.9274996255970764</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>4.6811246443172223</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="9"/>
+        <v>0.24637498127985413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>33.747</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>2.8330000000000002</v>
+      </c>
+      <c r="F16">
+        <v>1.482</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="8"/>
+        <v>4.6811246443172223</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>2.3263520602662253</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="9"/>
+        <v>2.354772584050997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <f>B16</f>
+        <v>33.747</v>
+      </c>
+      <c r="C17">
+        <v>-15</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>2.3392313239218812</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>1.482</v>
+      </c>
+      <c r="F17">
+        <v>1.482</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="8"/>
+        <v>2.3263520602662253</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="5"/>
+        <v>2.210034457252914</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="9"/>
+        <v>0.11631760301331129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: new m2_q optimization
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\LCLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SLAC\SLAC-Diling\11. 21 Winter\DXS_optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC6409-969E-4F1A-BC0D-AAE02144EE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F6645F-023C-4973-90F5-D37BB03C30FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="729" firstSheet="4" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="6876" yWindow="2436" windowWidth="17280" windowHeight="9024" tabRatio="729" firstSheet="4" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="86">
   <si>
     <t>E (eV)</t>
   </si>
@@ -341,14 +341,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -356,7 +356,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -364,13 +364,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -492,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -506,7 +506,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -514,19 +514,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -571,7 +571,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,7 +587,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -889,14 +889,14 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="24" t="s">
@@ -927,7 +927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -948,7 +948,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -969,7 +969,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1038,12 +1038,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -1053,7 +1053,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -1069,7 +1069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>99.95527741082276</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>14.788565117888117</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>24.624812898155728</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>6.6366999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0.54164665624999997</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>2.7082332812500054E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>0.51456432343749992</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -1319,7 +1319,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -1341,7 +1341,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0.39327210149576941</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>1.9663605074788482E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>0.37360849642098093</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>9.4726865189069517E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>62445196438317.109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="C43" s="9" t="s">
         <v>44</v>
       </c>
@@ -1724,14 +1724,14 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="24" t="s">
@@ -1762,7 +1762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1873,12 +1873,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -1888,7 +1888,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -1904,7 +1904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>Si(333)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>49.97763870541138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>1.3096054846052845</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>2.0933244980841712</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>1.3096054846052845</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>0.10049860000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>0.41010389687500004</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>2.0505194843750019E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>0.38959870203125002</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>1.1521811757211999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="47" t="s">
@@ -2178,7 +2178,7 @@
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19" t="s">
@@ -2200,7 +2200,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="16" t="s">
         <v>17</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="18" t="s">
         <v>20</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="16" t="s">
         <v>21</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="18" t="s">
         <v>23</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="16" t="s">
         <v>24</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="18" t="s">
         <v>25</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="16" t="s">
         <v>26</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="18" t="s">
         <v>27</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
         <v>28</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>0.19663605074788473</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="30" t="s">
         <v>29</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>9.8318025373942408E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="16" t="s">
         <v>30</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>0.18680424821049049</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>40</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>42</v>
       </c>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="C42" s="9" t="s">
         <v>43</v>
       </c>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="F42" s="8"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="C44" s="9" t="s">
         <v>44</v>
       </c>
@@ -2569,19 +2569,19 @@
       <selection activeCell="A14" sqref="A14:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>111</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>1.1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>220</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>5.8E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>400</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>2.4000000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>440</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>9.3000000000000007E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>311</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>23.541</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>331</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>31.66</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>333</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1.06E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>9481</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>6.1992700000000005E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>13.52792563251503</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>2.1831705598697404E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>2.0740120318762545E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>1.9703114302824398E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>12.801562343436874</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>5.8149870052605301E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>0.74393067087299591</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>1.8045843006325168E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="B31" t="s">
         <v>83</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>-1.1375067569572901E-18</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>142.46559719211601</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>12.568962863226453</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0.21709284819639318</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>0.81758717293962924</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>1.8045843006325168E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="B41" t="s">
         <v>83</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>-3.6051209103971797E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="B42" t="s">
         <v>84</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>213.240960670487</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>11.850760959418839</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>0.30339949743236461</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>1.4457996024079409</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>1.822998426149175E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="B51" t="s">
         <v>83</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>-2.5223707918536498E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="B52" t="s">
         <v>84</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>223.86280141900701</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>10.230725983216434</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>0.52008427636523091</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>2.8454669745741481</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>1.8414125516658331E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="B61" t="s">
         <v>83</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>-1.1375067569572901E-18</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="B62" t="s">
         <v>84</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>223.86280141900701</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>6.2479699711923846</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>0.63005894288577124</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>6.7182483200776559</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>1.8414125516658331E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9">
       <c r="B71" t="s">
         <v>83</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>6.77647058825995E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9">
       <c r="B72" t="s">
         <v>84</v>
       </c>
@@ -4272,26 +4272,26 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DF6462-A788-4188-BCB4-115117FE54BC}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>30.865652149480191</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>0.26171739252599036</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>2.9497988079516717</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>0.10114158250210736</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>0.13218848271986561</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>8.9475079241009059E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>23.177944647372861</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>0.64610276763135843</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>7.3484529593987054</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>0.24637498127985413</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>2.354772584050997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -4761,6 +4761,243 @@
       <c r="I17">
         <f t="shared" si="9"/>
         <v>0.11631760301331129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22">
+        <v>6.38</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f>SIN(RADIANS(B22-C22))/SIN(RADIANS(B22+C22))</f>
+        <v>0.36174591529536387</v>
+      </c>
+      <c r="E22">
+        <v>17.795000000000002</v>
+      </c>
+      <c r="F22">
+        <v>4.4619999999999997</v>
+      </c>
+      <c r="G22">
+        <f>40*0.95^2</f>
+        <v>36.1</v>
+      </c>
+      <c r="H22">
+        <f>G22*F22/E22*0.95</f>
+        <v>8.5992857544254004</v>
+      </c>
+      <c r="I22">
+        <f>G22-H22</f>
+        <v>27.500714245574599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23">
+        <f>B22</f>
+        <v>6.38</v>
+      </c>
+      <c r="C23">
+        <f>-C22</f>
+        <v>-3</v>
+      </c>
+      <c r="D23">
+        <f>SIN(RADIANS(B23-C23))/SIN(RADIANS(B23+C23))</f>
+        <v>2.764371227753891</v>
+      </c>
+      <c r="E23">
+        <f>F22</f>
+        <v>4.4619999999999997</v>
+      </c>
+      <c r="F23">
+        <v>4.4619999999999997</v>
+      </c>
+      <c r="G23">
+        <f>H22</f>
+        <v>8.5992857544254004</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H27" si="10">G23*F23/E23*0.95</f>
+        <v>8.1693214667041296</v>
+      </c>
+      <c r="I23">
+        <f>G23-H23</f>
+        <v>0.42996428772127082</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>10.454000000000001</v>
+      </c>
+      <c r="C24">
+        <v>7.5</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D27" si="11">SIN(RADIANS(B24-C24))/SIN(RADIANS(B24+C24))</f>
+        <v>0.16718128232162724</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E27" si="12">F23</f>
+        <v>4.4619999999999997</v>
+      </c>
+      <c r="F24">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G27" si="13">H23</f>
+        <v>8.1693214667041296</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="10"/>
+        <v>5.1031711618432141</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ref="I24:I27" si="14">G24-H24</f>
+        <v>3.0661503048609156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25">
+        <f>B24</f>
+        <v>10.454000000000001</v>
+      </c>
+      <c r="C25">
+        <f>-C24</f>
+        <v>-7.5</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="11"/>
+        <v>5.9815308634621944</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="12"/>
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="F25">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="13"/>
+        <v>5.1031711618432141</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="10"/>
+        <v>4.8480126037510534</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="14"/>
+        <v>0.2551585580921607</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26">
+        <v>33.747</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="12"/>
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="F26">
+        <v>0.23</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="13"/>
+        <v>4.8480126037510534</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="10"/>
+        <v>0.36103979342863163</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="14"/>
+        <v>4.4869728103224213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27">
+        <f>B26</f>
+        <v>33.747</v>
+      </c>
+      <c r="C27">
+        <v>-15</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="11"/>
+        <v>2.3392313239218812</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="12"/>
+        <v>0.23</v>
+      </c>
+      <c r="F27">
+        <v>0.23</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="13"/>
+        <v>0.36103979342863163</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="10"/>
+        <v>0.3429878037572</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="14"/>
+        <v>1.8051989671431623E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4778,12 +5015,12 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4795,7 +5032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -4814,7 +5051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -4835,7 +5072,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -4856,7 +5093,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -4878,7 +5115,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -4897,7 +5134,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -4925,12 +5162,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="49" t="s">
@@ -4940,7 +5177,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -4956,7 +5193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -4976,7 +5213,7 @@
         <v>Si(220)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -4995,7 +5232,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -5020,7 +5257,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -5046,7 +5283,7 @@
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -5068,7 +5305,7 @@
         <v>14.788565117888117</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -5090,7 +5327,7 @@
         <v>24.624812898155728</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -5112,7 +5349,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -5134,7 +5371,7 @@
         <v>3.6027799999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -5156,7 +5393,7 @@
         <v>0.29403675624999992</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="13" t="s">
         <v>29</v>
       </c>
@@ -5178,7 +5415,7 @@
         <v>1.4701837812500007E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -5200,12 +5437,12 @@
         <v>0.27933491843749991</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -5215,7 +5452,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -5231,7 +5468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -5252,7 +5489,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -5271,7 +5508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -5293,7 +5530,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -5315,7 +5552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -5337,7 +5574,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -5359,7 +5596,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -5381,7 +5618,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -5403,7 +5640,7 @@
         <v>3.6027799999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -5425,7 +5662,7 @@
         <v>0.23949477569535141</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="18" t="s">
         <v>29</v>
       </c>
@@ -5447,7 +5684,7 @@
         <v>1.1974738784767569E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -5469,7 +5706,7 @@
         <v>0.22752003691058384</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -5477,7 +5714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -5486,7 +5723,7 @@
         <v>2.5260497383751867E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -5514,12 +5751,12 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5531,7 +5768,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -5550,7 +5787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -5571,7 +5808,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -5592,7 +5829,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -5614,7 +5851,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="34" customFormat="1">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -5633,7 +5870,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -5661,12 +5898,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="49" t="s">
@@ -5676,7 +5913,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -5692,7 +5929,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -5710,7 +5947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -5728,7 +5965,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -5753,7 +5990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -5779,7 +6016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -5801,7 +6038,7 @@
         <v>14.788565117888117</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -5823,7 +6060,7 @@
         <v>24.624812898155728</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -5845,7 +6082,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -5867,7 +6104,7 @@
         <v>6.6366999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -5889,7 +6126,7 @@
         <v>16.926458007812499</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="34" customFormat="1">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -5911,7 +6148,7 @@
         <v>0.84632290039062497</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -5933,12 +6170,12 @@
         <v>16.080135107421874</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -5948,7 +6185,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -5970,7 +6207,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -5993,7 +6230,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -6018,7 +6255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -6046,7 +6283,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -6074,7 +6311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -6104,7 +6341,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -6134,7 +6371,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -6164,7 +6401,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -6194,7 +6431,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -6224,7 +6461,7 @@
         <v>9.7778322860450473</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="34" customFormat="1">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -6253,7 +6490,7 @@
         <v>0.48889161430225236</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -6283,7 +6520,7 @@
         <v>9.2889406717427949</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -6291,7 +6528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -6300,7 +6537,7 @@
         <v>0.78939054324224611</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -6328,12 +6565,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6345,7 +6582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -6364,7 +6601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -6385,7 +6622,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -6406,7 +6643,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -6428,7 +6665,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="34" customFormat="1">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -6447,7 +6684,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -6475,12 +6712,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="49" t="s">
@@ -6490,7 +6727,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -6506,7 +6743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -6526,7 +6763,7 @@
         <v>Si(220)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -6545,7 +6782,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -6570,7 +6807,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -6596,7 +6833,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -6618,7 +6855,7 @@
         <v>14.788565117888117</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -6640,7 +6877,7 @@
         <v>24.624812898155728</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -6662,7 +6899,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -6684,7 +6921,7 @@
         <v>3.6027799999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -6706,7 +6943,7 @@
         <v>9.1886486328124963</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="34" customFormat="1">
       <c r="A21" s="13" t="s">
         <v>29</v>
       </c>
@@ -6728,7 +6965,7 @@
         <v>0.45943243164062508</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -6750,12 +6987,12 @@
         <v>8.7292162011718712</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -6765,7 +7002,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -6781,7 +7018,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -6802,7 +7039,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -6821,7 +7058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -6843,7 +7080,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -6865,7 +7102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -6887,7 +7124,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -6909,7 +7146,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -6931,7 +7168,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -6953,7 +7190,7 @@
         <v>3.6027799999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -6975,7 +7212,7 @@
         <v>7.484211740479731</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="34" customFormat="1">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -6997,7 +7234,7 @@
         <v>0.37421058702398557</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -7019,7 +7256,7 @@
         <v>7.1100011534557455</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -7027,7 +7264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -7036,7 +7273,7 @@
         <v>0.78939054324224578</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -7064,14 +7301,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7083,7 +7320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="24" t="s">
@@ -7102,7 +7339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -7123,7 +7360,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -7144,7 +7381,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -7166,7 +7403,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -7185,7 +7422,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -7213,12 +7450,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -7228,7 +7465,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -7244,7 +7481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -7264,7 +7501,7 @@
         <v>Si(111)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -7283,7 +7520,7 @@
         <v>-9.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -7308,7 +7545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -7334,7 +7571,7 @@
         <v>49.97763870541138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -7356,7 +7593,7 @@
         <v>8.7997821753981018</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -7378,7 +7615,7 @@
         <v>24.404323473920872</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -7400,7 +7637,7 @@
         <v>1.2499999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -7422,7 +7659,7 @@
         <v>0.227544</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -7444,7 +7681,7 @@
         <v>0.92853712499999974</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -7466,7 +7703,7 @@
         <v>4.6426856249999982E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -7488,7 +7725,7 @@
         <v>0.88211026874999976</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -7498,7 +7735,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -7520,7 +7757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -7543,7 +7780,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -7568,7 +7805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -7596,7 +7833,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -7624,7 +7861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -7654,7 +7891,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -7684,7 +7921,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -7714,7 +7951,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -7744,7 +7981,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -7774,7 +8011,7 @@
         <v>0.19663605074788468</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -7803,7 +8040,7 @@
         <v>9.8318025373942408E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -7833,7 +8070,7 @@
         <v>0.18680424821049044</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -7841,7 +8078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -7851,7 +8088,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -7861,7 +8098,7 @@
       </c>
       <c r="F41" s="8"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="C43" s="9" t="s">
         <v>44</v>
       </c>
@@ -7888,14 +8125,14 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7907,7 +8144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="24" t="s">
@@ -7926,7 +8163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -7947,7 +8184,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -7968,7 +8205,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -7990,7 +8227,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -8009,7 +8246,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -8037,12 +8274,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -8052,7 +8289,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -8068,7 +8305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -8088,7 +8325,7 @@
         <v>Si(111)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -8107,7 +8344,7 @@
         <v>-9.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -8132,7 +8369,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -8158,7 +8395,7 @@
         <v>99.95527741082276</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -8180,7 +8417,7 @@
         <v>8.7997821753981018</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -8202,7 +8439,7 @@
         <v>24.404323473920872</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -8224,7 +8461,7 @@
         <v>1.2499999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -8246,7 +8483,7 @@
         <v>0.39306636024274866</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -8268,7 +8505,7 @@
         <v>4.4879294374999992</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -8290,7 +8527,7 @@
         <v>1.4403617348111544</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -8312,7 +8549,7 @@
         <v>3.0475677026888448</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -8322,7 +8559,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -8344,7 +8581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -8367,7 +8604,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -8392,7 +8629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -8420,7 +8657,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -8448,7 +8685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -8478,7 +8715,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -8508,7 +8745,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -8538,7 +8775,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -8568,7 +8805,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -8598,7 +8835,7 @@
         <v>0.39327210149576936</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -8627,7 +8864,7 @@
         <v>1.9663605074788482E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -8657,7 +8894,7 @@
         <v>0.37360849642098087</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -8665,7 +8902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -8675,7 +8912,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -8685,7 +8922,7 @@
       </c>
       <c r="F41" s="8"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="C43" s="9" t="s">
         <v>44</v>
       </c>
@@ -8712,12 +8949,12 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8729,7 +8966,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -8748,7 +8985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -8769,7 +9006,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -8790,7 +9027,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -8812,7 +9049,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="34" customFormat="1">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -8831,7 +9068,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -8859,12 +9096,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="49" t="s">
@@ -8874,7 +9111,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -8890,7 +9127,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -8910,7 +9147,7 @@
         <v>Si(111)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -8929,7 +9166,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -8954,7 +9191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -8980,7 +9217,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -9002,7 +9239,7 @@
         <v>8.4717585570273428</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -9024,7 +9261,7 @@
         <v>23.601207524361531</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -9046,7 +9283,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -9068,7 +9305,7 @@
         <v>0.227544</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -9090,7 +9327,7 @@
         <v>3.2424613561648532</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="34" customFormat="1">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -9112,7 +9349,7 @@
         <v>0.16212306780824282</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -9134,7 +9371,7 @@
         <v>3.0803382883566104</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -9144,7 +9381,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -9166,7 +9403,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -9189,7 +9426,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -9214,7 +9451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -9242,7 +9479,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -9270,7 +9507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -9300,7 +9537,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -9330,7 +9567,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -9360,7 +9597,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -9390,7 +9627,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -9420,7 +9657,7 @@
         <v>-2.4359551087418119</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="34" customFormat="1">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -9449,7 +9686,7 @@
         <v>-0.12179775543709059</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -9479,7 +9716,7 @@
         <v>-2.3141573533047213</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -9487,7 +9724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -9496,7 +9733,7 @@
         <v>4.4104960587504155E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -9524,14 +9761,14 @@
       <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9543,7 +9780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="24" t="s">
@@ -9562,7 +9799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -9583,7 +9820,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -9604,7 +9841,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -9626,7 +9863,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -9645,7 +9882,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -9673,12 +9910,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -9688,7 +9925,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -9704,7 +9941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -9724,7 +9961,7 @@
         <v>Si(111)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -9744,7 +9981,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -9767,7 +10004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -9793,7 +10030,7 @@
         <v>49.97763870541138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -9815,7 +10052,7 @@
         <v>8.8581423094935765</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -9836,7 +10073,7 @@
         <v>24.669784419999996</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -9858,7 +10095,7 @@
         <v>1.3096054846052845</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -9880,7 +10117,7 @@
         <v>7.9472748360726694E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -9902,7 +10139,7 @@
         <v>0.32430385894032632</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -9924,7 +10161,7 @@
         <v>1.6215192947016344E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -9946,7 +10183,7 @@
         <v>0.30808866599330997</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="47" t="s">
@@ -9956,7 +10193,7 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -9978,7 +10215,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>17</v>
       </c>
@@ -10001,7 +10238,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>20</v>
       </c>
@@ -10026,7 +10263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>21</v>
       </c>
@@ -10054,7 +10291,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
@@ -10082,7 +10319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -10112,7 +10349,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
@@ -10142,7 +10379,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -10172,7 +10409,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
@@ -10202,7 +10439,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -10232,7 +10469,7 @@
         <v>0.19663605074788465</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="30" t="s">
         <v>29</v>
       </c>
@@ -10261,7 +10498,7 @@
         <v>9.8318025373942408E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>30</v>
       </c>
@@ -10291,7 +10528,7 @@
         <v>0.18680424821049041</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="C39" s="9" t="s">
         <v>40</v>
       </c>
@@ -10299,7 +10536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
@@ -10309,7 +10546,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
@@ -10319,7 +10556,7 @@
       </c>
       <c r="F41" s="8"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="C43" s="9" t="s">
         <v>44</v>
       </c>
@@ -10346,15 +10583,15 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10366,7 +10603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="24" t="s">
@@ -10385,7 +10622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -10406,7 +10643,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -10427,7 +10664,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -10449,7 +10686,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
@@ -10468,7 +10705,7 @@
       </c>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -10496,12 +10733,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="46" t="s">
@@ -10511,7 +10748,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12" t="s">
@@ -10527,7 +10764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -10547,7 +10784,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
@@ -10567,7 +10804,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -10590,7 +10827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -10616,7 +10853,7 @@
         <v>49.97763870541138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -10638,7 +10875,7 @@
         <v>1.6120252845656888</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -10659,7 +10896,7 @@
         <v>2.1546945457960813</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -10681,7 +10918,7 @@
         <v>1.3096054846052845</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -10699,7 +10936,7 @@
         <v>0.107</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -10725,7 +10962,7 @@
         <v>11.827956989247312</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
@@ -10747,7 +10984,7 @@
         <v>2.1831705598697404E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -10773,7 +11010,7 @@
         <v>3.9677836197446896</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
@@ -10795,7 +11032,7 @@
         <v>1.40159556457608</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="47" t="s">
@@ -10805,7 +11042,7 @@
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19" t="s">
@@ -10827,7 +11064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="16" t="s">
         <v>17</v>
       </c>
@@ -10850,7 +11087,7 @@
         <v>Si(440)</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="18" t="s">
         <v>20</v>
       </c>
@@ -10875,7 +11112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="16" t="s">
         <v>21</v>
       </c>
@@ -10903,7 +11140,7 @@
         <v>42.927866251322122</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="18" t="s">
         <v>23</v>
       </c>
@@ -10931,7 +11168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="16" t="s">
         <v>24</v>
       </c>
@@ -10961,7 +11198,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="18" t="s">
         <v>25</v>
       </c>
@@ -10991,7 +11228,7 @@
         <v>1.8353282787546381</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="16" t="s">
         <v>26</v>
       </c>
@@ -11021,7 +11258,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="18" t="s">
         <v>27</v>
       </c>
@@ -11051,7 +11288,7 @@
         <v>6.555225368123066E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
         <v>28</v>
       </c>
@@ -11081,7 +11318,7 @@
         <v>0.19663605074788473</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="30" t="s">
         <v>29</v>
       </c>
@@ -11110,7 +11347,7 @@
         <v>9.8318025373942408E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="16" t="s">
         <v>30</v>
       </c>
@@ -11140,7 +11377,7 @@
         <v>0.18680424821049049</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" s="9" t="s">
         <v>40</v>
       </c>
@@ -11148,7 +11385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="C41" s="9" t="s">
         <v>42</v>
       </c>
@@ -11158,7 +11395,7 @@
       </c>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="C42" s="9" t="s">
         <v>43</v>
       </c>
@@ -11168,7 +11405,7 @@
       </c>
       <c r="F42" s="8"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="C44" s="9" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Update: m2_q optimization for higher powers
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SLAC\SLAC-Diling\11. 21 Winter\DXS_optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F6645F-023C-4973-90F5-D37BB03C30FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE613A29-20D9-4882-880B-800E11295019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6876" yWindow="2436" windowWidth="17280" windowHeight="9024" tabRatio="729" firstSheet="4" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="1452" yWindow="2004" windowWidth="17280" windowHeight="9024" tabRatio="729" firstSheet="4" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -4275,7 +4275,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
Update: m2_q optimization for 9481eV from 100% to 50% power
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SLAC\SLAC-Diling\11. 21 Winter\DXS_optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE613A29-20D9-4882-880B-800E11295019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C31D563-E7A5-4F12-8AEE-97C6F64818C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="2004" windowWidth="17280" windowHeight="9024" tabRatio="729" firstSheet="4" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="-16297" yWindow="15" windowWidth="16395" windowHeight="28050" tabRatio="729" firstSheet="6" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="zig-zag_power_calc" sheetId="10" r:id="rId8"/>
     <sheet name="2DCM-111-440" sheetId="11" r:id="rId9"/>
     <sheet name="2DCM-111-333" sheetId="12" r:id="rId10"/>
-    <sheet name="bw factor" sheetId="13" r:id="rId11"/>
-    <sheet name="17795" sheetId="14" r:id="rId12"/>
+    <sheet name="9482-2DCM" sheetId="13" r:id="rId11"/>
+    <sheet name="9481-Zig" sheetId="15" r:id="rId12"/>
+    <sheet name="17795" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="86">
   <si>
     <t>E (eV)</t>
   </si>
@@ -885,18 +886,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54856E7F-A460-AD4D-A5A7-16FDBABB0388}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1724,14 +1725,14 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2566,18 +2567,18 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I20"/>
+      <selection activeCell="A64" sqref="A64:I70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4271,23 +4272,279 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A8719F-33BE-4F0E-9559-A6EEE68C0B3D}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>12.042523880204399</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <f>SIN(RADIANS(B2-C2))/SIN(RADIANS(B2+C2))</f>
+        <v>0.14782208373497599</v>
+      </c>
+      <c r="E2">
+        <f>9481/1000</f>
+        <v>9.4809999999999999</v>
+      </c>
+      <c r="F2">
+        <v>3.35</v>
+      </c>
+      <c r="G2">
+        <f>50*0.95^2</f>
+        <v>45.125</v>
+      </c>
+      <c r="H2">
+        <f>G2*F2/E2*0.95</f>
+        <v>15.147169338677356</v>
+      </c>
+      <c r="I2">
+        <f>G2-H2</f>
+        <v>29.977830661322642</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>19.9159058696595</v>
+      </c>
+      <c r="C3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="0">SIN(RADIANS(B3-C3))/SIN(RADIANS(B3+C3))</f>
+        <v>8.7798992905339462E-2</v>
+      </c>
+      <c r="E3">
+        <f>F2</f>
+        <v>3.35</v>
+      </c>
+      <c r="F3">
+        <v>3.355</v>
+      </c>
+      <c r="G3">
+        <f>H2</f>
+        <v>15.147169338677356</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="1">G3*F3/E3*0.95</f>
+        <v>14.411288201402806</v>
+      </c>
+      <c r="I3">
+        <f>G3-H3</f>
+        <v>0.73588113727454996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <f>B3</f>
+        <v>19.9159058696595</v>
+      </c>
+      <c r="C4">
+        <f>-C3</f>
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>11.389652283120727</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E7" si="2">F3</f>
+        <v>3.355</v>
+      </c>
+      <c r="F4">
+        <v>3.35</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G7" si="3">H3</f>
+        <v>14.411288201402806</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>13.670320328156313</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I7" si="4">G4-H4</f>
+        <v>0.74096787324649327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <f>B2</f>
+        <v>12.042523880204399</v>
+      </c>
+      <c r="C5">
+        <f>-C2</f>
+        <v>-9</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>6.7648890797186843</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>3.35</v>
+      </c>
+      <c r="F5">
+        <v>3.0920000000000001</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>13.670320328156313</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>11.986626546843688</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>1.6836937813126251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6">
+        <v>42.928413263468897</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>3.0920000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>11.986626546843688</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>1.0790677552761772</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>10.90755879156751</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
+        <f>B6</f>
+        <v>42.928413263468897</v>
+      </c>
+      <c r="C7">
+        <v>-15</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.8092297153788244</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1.0790677552761772</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.60877098958072384</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>0.47029676569545331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DF6462-A788-4188-BCB4-115117FE54BC}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5015,12 +5272,12 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.8984375" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5747,16 +6004,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888623A0-050A-CC41-A2E3-B9B041ACA338}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.8984375" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6565,12 +6822,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.8984375" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7301,14 +7558,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8125,14 +8382,14 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8946,15 +9203,15 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.8984375" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9758,17 +10015,17 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10583,15 +10840,15 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update: m2_p optimization for 9481 Zigzag/2DCM-111-220
The 2D phase structure for m2_p correction is not quite right...
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SLAC\SLAC-Diling\11. 21 Winter\DXS_optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C31D563-E7A5-4F12-8AEE-97C6F64818C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E815E605-4BFF-40C5-9F14-15E46A97F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16297" yWindow="15" windowWidth="16395" windowHeight="28050" tabRatio="729" firstSheet="6" activeTab="11" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" tabRatio="729" firstSheet="6" activeTab="10" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="zig-zag_power_calc" sheetId="10" r:id="rId8"/>
     <sheet name="2DCM-111-440" sheetId="11" r:id="rId9"/>
     <sheet name="2DCM-111-333" sheetId="12" r:id="rId10"/>
-    <sheet name="9482-2DCM" sheetId="13" r:id="rId11"/>
+    <sheet name="9481-2DCM" sheetId="13" r:id="rId11"/>
     <sheet name="9481-Zig" sheetId="15" r:id="rId12"/>
     <sheet name="17795" sheetId="14" r:id="rId13"/>
   </sheets>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="86">
   <si>
     <t>E (eV)</t>
   </si>
@@ -2564,22 +2564,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD56799-D342-4B40-B7BD-BBBEDC8F0C10}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:I70"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3668,7 +3673,7 @@
         <v>0.30339949743236461</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -3703,7 +3708,7 @@
         <v>1.4457996024079409</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -3738,7 +3743,7 @@
         <v>1.822998426149175E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:19">
       <c r="B51" t="s">
         <v>83</v>
       </c>
@@ -3746,7 +3751,7 @@
         <v>-2.5223707918536498E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:19">
       <c r="B52" t="s">
         <v>84</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>223.86280141900701</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -3783,7 +3788,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3817,7 +3822,7 @@
         <v>29.977830661322642</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -3853,7 +3858,7 @@
         <v>1.1826095941883779</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>10.230725983216434</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:19">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -3923,7 +3928,7 @@
         <v>0.52008427636523091</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -3958,7 +3963,7 @@
         <v>2.8454669745741481</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -3993,7 +3998,7 @@
         <v>1.8414125516658331E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:19">
       <c r="B61" t="s">
         <v>83</v>
       </c>
@@ -4001,7 +4006,7 @@
         <v>-1.1375067569572901E-18</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:19">
       <c r="B62" t="s">
         <v>84</v>
       </c>
@@ -4009,7 +4014,7 @@
         <v>223.86280141900701</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:19">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -4037,8 +4042,35 @@
       <c r="I64" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="K64" t="s">
+        <v>82</v>
+      </c>
+      <c r="L64" t="s">
+        <v>70</v>
+      </c>
+      <c r="M64" t="s">
+        <v>71</v>
+      </c>
+      <c r="N64" t="s">
+        <v>73</v>
+      </c>
+      <c r="O64" t="s">
+        <v>76</v>
+      </c>
+      <c r="P64" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>74</v>
+      </c>
+      <c r="R64" t="s">
+        <v>77</v>
+      </c>
+      <c r="S64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -4057,7 +4089,7 @@
         <v>9.4809999999999999</v>
       </c>
       <c r="F65">
-        <v>3.35</v>
+        <v>3.355</v>
       </c>
       <c r="G65">
         <f>50*0.95^2</f>
@@ -4065,14 +4097,45 @@
       </c>
       <c r="H65">
         <f>G65*F65/E65*0.95</f>
-        <v>15.147169338677356</v>
+        <v>15.169777054108215</v>
       </c>
       <c r="I65">
         <f>G65-H65</f>
-        <v>29.977830661322642</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>29.955222945891784</v>
+      </c>
+      <c r="K65" t="s">
+        <v>64</v>
+      </c>
+      <c r="L65">
+        <v>12.0368582999333</v>
+      </c>
+      <c r="M65">
+        <v>9</v>
+      </c>
+      <c r="N65">
+        <f>SIN(RADIANS(L65-M65))/SIN(RADIANS(L65+M65))</f>
+        <v>0.14758501191458828</v>
+      </c>
+      <c r="O65">
+        <v>9.4809999999999999</v>
+      </c>
+      <c r="P65">
+        <v>3.355</v>
+      </c>
+      <c r="Q65">
+        <f>50*0.95^2</f>
+        <v>45.125</v>
+      </c>
+      <c r="R65">
+        <f>Q65*P65/O65*0.95</f>
+        <v>15.169777054108215</v>
+      </c>
+      <c r="S65">
+        <f>Q65-R65</f>
+        <v>29.955222945891784</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -4090,25 +4153,59 @@
       </c>
       <c r="E66">
         <f>F65</f>
-        <v>3.35</v>
+        <v>3.355</v>
       </c>
       <c r="F66">
-        <v>3.2509999999999999</v>
+        <v>3.2789999999999999</v>
       </c>
       <c r="G66">
         <f>H65</f>
-        <v>15.147169338677356</v>
+        <v>15.169777054108215</v>
       </c>
       <c r="H66">
         <f t="shared" ref="H66:H70" si="28">G66*F66/E66*0.95</f>
-        <v>13.964559744488978</v>
+        <v>14.084832790581158</v>
       </c>
       <c r="I66">
         <f>G66-H66</f>
-        <v>1.1826095941883779</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>1.0849442635270563</v>
+      </c>
+      <c r="K66" t="s">
+        <v>66</v>
+      </c>
+      <c r="L66">
+        <f>L65</f>
+        <v>12.0368582999333</v>
+      </c>
+      <c r="M66">
+        <f>-M65</f>
+        <v>-9</v>
+      </c>
+      <c r="N66">
+        <f>SIN(RADIANS(L66-M66))/SIN(RADIANS(L66+M66))</f>
+        <v>6.7757557967927591</v>
+      </c>
+      <c r="O66">
+        <f>P65</f>
+        <v>3.355</v>
+      </c>
+      <c r="P66">
+        <v>3.2789999999999999</v>
+      </c>
+      <c r="Q66">
+        <f>R65</f>
+        <v>15.169777054108215</v>
+      </c>
+      <c r="R66">
+        <f t="shared" ref="R66:R70" si="29">Q66*P66/O66*0.95</f>
+        <v>14.084832790581158</v>
+      </c>
+      <c r="S66">
+        <f>Q66-R66</f>
+        <v>1.0849442635270563</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -4119,30 +4216,62 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D70" si="29">SIN(RADIANS(B67-C67))/SIN(RADIANS(B67+C67))</f>
+        <f t="shared" ref="D67:D70" si="30">SIN(RADIANS(B67-C67))/SIN(RADIANS(B67+C67))</f>
         <v>8.7639288616412861E-2</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E70" si="30">F66</f>
-        <v>3.2509999999999999</v>
+        <f t="shared" ref="E67:E70" si="31">F66</f>
+        <v>3.2789999999999999</v>
       </c>
       <c r="F67">
-        <v>1.891</v>
+        <v>1.887</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G70" si="31">H66</f>
-        <v>13.964559744488978</v>
+        <f t="shared" ref="G67:G70" si="32">H66</f>
+        <v>14.084832790581158</v>
       </c>
       <c r="H67">
         <f t="shared" si="28"/>
-        <v>7.7165897732965938</v>
+        <v>7.700267002755508</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I70" si="32">G67-H67</f>
-        <v>6.2479699711923846</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <f t="shared" ref="I67:I70" si="33">G67-H67</f>
+        <v>6.3845657878256503</v>
+      </c>
+      <c r="K67" t="s">
+        <v>67</v>
+      </c>
+      <c r="L67">
+        <v>19.91</v>
+      </c>
+      <c r="M67">
+        <v>13</v>
+      </c>
+      <c r="N67">
+        <f t="shared" ref="N67:N70" si="34">SIN(RADIANS(L67-M67))/SIN(RADIANS(L67+M67))</f>
+        <v>0.22143467602751127</v>
+      </c>
+      <c r="O67">
+        <f t="shared" ref="O67:O70" si="35">P66</f>
+        <v>3.2789999999999999</v>
+      </c>
+      <c r="P67">
+        <v>1.206</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" ref="Q67:Q70" si="36">R66</f>
+        <v>14.084832790581158</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="29"/>
+        <v>4.9213153181362701</v>
+      </c>
+      <c r="S67">
+        <f t="shared" ref="S67:S70" si="37">Q67-R67</f>
+        <v>9.1635174724448873</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -4155,30 +4284,64 @@
         <v>-16.899999999999999</v>
       </c>
       <c r="D68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>11.410407544233792</v>
       </c>
       <c r="E68">
-        <f t="shared" si="30"/>
-        <v>1.891</v>
+        <f t="shared" si="31"/>
+        <v>1.887</v>
       </c>
       <c r="F68">
-        <v>1.8280000000000001</v>
+        <v>1.7749999999999999</v>
       </c>
       <c r="G68">
-        <f t="shared" si="31"/>
-        <v>7.7165897732965938</v>
+        <f t="shared" si="32"/>
+        <v>7.700267002755508</v>
       </c>
       <c r="H68">
         <f t="shared" si="28"/>
-        <v>7.0865308304108225</v>
+        <v>6.881067956224947</v>
       </c>
       <c r="I68">
-        <f t="shared" si="32"/>
-        <v>0.63005894288577124</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <f t="shared" si="33"/>
+        <v>0.81919904653056097</v>
+      </c>
+      <c r="K68" t="s">
+        <v>65</v>
+      </c>
+      <c r="L68">
+        <f>L67</f>
+        <v>19.91</v>
+      </c>
+      <c r="M68">
+        <f>-M67</f>
+        <v>-13</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="34"/>
+        <v>4.5160045298224158</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="35"/>
+        <v>1.206</v>
+      </c>
+      <c r="P68">
+        <v>1.1930000000000001</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="36"/>
+        <v>4.9213153181362701</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="29"/>
+        <v>4.6248529981838651</v>
+      </c>
+      <c r="S68">
+        <f t="shared" si="37"/>
+        <v>0.29646231995240502</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4190,30 +4353,62 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="E69">
-        <f t="shared" si="30"/>
-        <v>1.8280000000000001</v>
+        <f t="shared" si="31"/>
+        <v>1.7749999999999999</v>
       </c>
       <c r="F69">
-        <v>0.1</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="G69">
-        <f t="shared" si="31"/>
-        <v>7.0865308304108225</v>
+        <f t="shared" si="32"/>
+        <v>6.881067956224947</v>
       </c>
       <c r="H69">
         <f t="shared" si="28"/>
-        <v>0.36828251033316639</v>
+        <v>1.0606536297595186</v>
       </c>
       <c r="I69">
-        <f t="shared" si="32"/>
-        <v>6.7182483200776559</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <f t="shared" si="33"/>
+        <v>5.8204143264654284</v>
+      </c>
+      <c r="K69" t="s">
+        <v>68</v>
+      </c>
+      <c r="L69">
+        <v>42.929010627216698</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="35"/>
+        <v>1.1930000000000001</v>
+      </c>
+      <c r="P69">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="36"/>
+        <v>4.6248529981838651</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="29"/>
+        <v>1.0459223293461914</v>
+      </c>
+      <c r="S69">
+        <f t="shared" si="37"/>
+        <v>3.5789306688376739</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -4225,43 +4420,60 @@
         <v>-15</v>
       </c>
       <c r="D70">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1.8092059522717598</v>
       </c>
       <c r="E70">
-        <f t="shared" si="30"/>
-        <v>0.1</v>
+        <f t="shared" si="31"/>
+        <v>0.28799999999999998</v>
       </c>
       <c r="F70">
-        <v>0.1</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="G70">
-        <f t="shared" si="31"/>
-        <v>0.36828251033316639</v>
+        <f t="shared" si="32"/>
+        <v>1.0606536297595186</v>
       </c>
       <c r="H70">
         <f t="shared" si="28"/>
-        <v>0.34986838481650806</v>
+        <v>0.60177362188439354</v>
       </c>
       <c r="I70">
-        <f t="shared" si="32"/>
-        <v>1.8414125516658331E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="B71" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71">
-        <v>6.77647058825995E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="B72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72">
-        <v>66.333555879288298</v>
+        <f t="shared" si="33"/>
+        <v>0.45888000787512506</v>
+      </c>
+      <c r="K70" t="s">
+        <v>69</v>
+      </c>
+      <c r="L70">
+        <f>L69</f>
+        <v>42.929010627216698</v>
+      </c>
+      <c r="M70">
+        <v>-15</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="34"/>
+        <v>1.8092059522717598</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="35"/>
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="P70">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="36"/>
+        <v>1.0459223293461914</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="29"/>
+        <v>0.59827493803622822</v>
+      </c>
+      <c r="S70">
+        <f t="shared" si="37"/>
+        <v>0.44764739130996323</v>
       </c>
     </row>
   </sheetData>
@@ -4273,15 +4485,22 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A8719F-33BE-4F0E-9559-A6EEE68C0B3D}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4520,6 +4739,244 @@
       <c r="I7">
         <f t="shared" si="4"/>
         <v>0.47029676569545331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>12.042523880204399</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f>SIN(RADIANS(B10-C10))/SIN(RADIANS(B10+C10))</f>
+        <v>0.14782208373497599</v>
+      </c>
+      <c r="E10">
+        <f>9481/1000</f>
+        <v>9.4809999999999999</v>
+      </c>
+      <c r="F10">
+        <v>3.35</v>
+      </c>
+      <c r="G10">
+        <f>50*0.95^2</f>
+        <v>45.125</v>
+      </c>
+      <c r="H10">
+        <f>G10*F10/E10*0.95</f>
+        <v>15.147169338677356</v>
+      </c>
+      <c r="I10">
+        <f>G10-H10</f>
+        <v>29.977830661322642</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11">
+        <v>19.9159058696595</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D15" si="5">SIN(RADIANS(B11-C11))/SIN(RADIANS(B11+C11))</f>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f>F10</f>
+        <v>3.35</v>
+      </c>
+      <c r="F11">
+        <v>1.149</v>
+      </c>
+      <c r="G11">
+        <f>H10</f>
+        <v>15.147169338677356</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H15" si="6">G11*F11/E11*0.95</f>
+        <v>4.9354903557114236</v>
+      </c>
+      <c r="I11">
+        <f>G11-H11</f>
+        <v>10.211678982965932</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <f>B11</f>
+        <v>19.9159058696595</v>
+      </c>
+      <c r="C12">
+        <f>-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E15" si="7">F11</f>
+        <v>1.149</v>
+      </c>
+      <c r="F12">
+        <v>1.149</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G15" si="8">H11</f>
+        <v>4.9354903557114236</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>4.6887158379258524</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I15" si="9">G12-H12</f>
+        <v>0.24677451778557113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13">
+        <f>B10</f>
+        <v>12.042523880204399</v>
+      </c>
+      <c r="C13">
+        <f>-C10</f>
+        <v>-9</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="5"/>
+        <v>6.7648890797186843</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="7"/>
+        <v>1.149</v>
+      </c>
+      <c r="F13">
+        <v>1.149</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="8"/>
+        <v>4.6887158379258524</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="6"/>
+        <v>4.4542800460295595</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="9"/>
+        <v>0.23443579189629293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14">
+        <v>42.928413263468897</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="7"/>
+        <v>1.149</v>
+      </c>
+      <c r="F14">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="8"/>
+        <v>4.4542800460295595</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>1.0422395042428607</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="9"/>
+        <v>3.4120405417866988</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15">
+        <f>B14</f>
+        <v>42.928413263468897</v>
+      </c>
+      <c r="C15">
+        <v>-15</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="5"/>
+        <v>1.8092297153788244</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="F15">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="8"/>
+        <v>1.0422395042428607</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>0.59827493803622878</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="9"/>
+        <v>0.44396456620663194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: debugging bending + phase corrector
</commit_message>
<xml_diff>
--- a/LCLS/power_calculation.xlsx
+++ b/LCLS/power_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SLAC\SLAC-Diling\11. 21 Winter\DXS_optics\LCLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E815E605-4BFF-40C5-9F14-15E46A97F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CCD208-79CA-4868-A253-139046E508CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" tabRatio="729" firstSheet="6" activeTab="10" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
+    <workbookView xWindow="120" yWindow="585" windowWidth="12615" windowHeight="20295" tabRatio="729" firstSheet="9" activeTab="10" xr2:uid="{6FDFD292-6916-AD47-BD4D-5B8A402B5A12}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE-HHLM-66meV" sheetId="1" r:id="rId1"/>
@@ -2566,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD56799-D342-4B40-B7BD-BBBEDC8F0C10}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
-      <selection activeCell="P73" sqref="P73"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4487,7 +4487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A8719F-33BE-4F0E-9559-A6EEE68C0B3D}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>